<commit_message>
Added JSON serialization for user profile. User can view their profile and update their first and last name. next steps are to link shirt with user.
</commit_message>
<xml_diff>
--- a/Docs/Specifications_FitMe.xlsx
+++ b/Docs/Specifications_FitMe.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\DLThrasher\Development\Projects Via Source Tree\Visual Studios\Website\FitMe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\DLThrasher\Development\Projects Via Source Tree\Visual Studios\Website\FitMe\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="Exceptions" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t xml:space="preserve">completion interval </t>
+  </si>
+  <si>
+    <t>0x0001</t>
+  </si>
+  <si>
+    <t>UserModel</t>
+  </si>
+  <si>
+    <t>When signing in we found repeat emails in DB</t>
+  </si>
+  <si>
+    <t>0x0002</t>
+  </si>
+  <si>
+    <t>Failure displaying user profile because user is incomplete</t>
+  </si>
+  <si>
+    <t>UserProfile.aspx</t>
   </si>
 </sst>
 </file>
@@ -397,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,6 +443,28 @@
       </c>
       <c r="C2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Show that user profile was successfully updated
</commit_message>
<xml_diff>
--- a/Docs/Specifications_FitMe.xlsx
+++ b/Docs/Specifications_FitMe.xlsx
@@ -25,20 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>When reading for the colum there was more than 1 id with the filtered value</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
     <t>TopModel</t>
   </si>
   <si>
@@ -64,6 +55,24 @@
   </si>
   <si>
     <t>UserProfile.aspx</t>
+  </si>
+  <si>
+    <t>0x0003</t>
+  </si>
+  <si>
+    <t>Database is not responding</t>
+  </si>
+  <si>
+    <t>DataBase.cs</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -415,56 +424,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +509,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>200</v>

</xml_diff>

<commit_message>
Made user rated item properties public so they get saved in the DB Reorganice nav bar so that the logout and profile is under my account Added property to DataBaseResult to say whether the id was found and if it is a new item then then both values get set to true!
</commit_message>
<xml_diff>
--- a/Docs/Specifications_FitMe.xlsx
+++ b/Docs/Specifications_FitMe.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>When reading for the colum there was more than 1 id with the filtered value</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>0x0004</t>
+  </si>
+  <si>
+    <t>0x0004, Failed to ReadFromTable,</t>
   </si>
 </sst>
 </file>
@@ -424,9 +430,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -487,6 +495,17 @@
       </c>
       <c r="C5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added User Closet to display clothes User can add the same item multiple times (need to block this) should prompt for udpates User can delete items from their closet (Validating column added to top table) Page permissions started
</commit_message>
<xml_diff>
--- a/Docs/Specifications_FitMe.xlsx
+++ b/Docs/Specifications_FitMe.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>When reading for the colum there was more than 1 id with the filtered value</t>
   </si>
@@ -78,7 +78,16 @@
     <t>0x0004</t>
   </si>
   <si>
-    <t>0x0004, Failed to ReadFromTable,</t>
+    <t>0x0005</t>
+  </si>
+  <si>
+    <t>TopModel.cs</t>
+  </si>
+  <si>
+    <t>Failed to ReadFromTable,</t>
+  </si>
+  <si>
+    <t>Try Removing Top Failed</t>
   </si>
 </sst>
 </file>
@@ -430,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +514,18 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing the star rating!
</commit_message>
<xml_diff>
--- a/Docs/Specifications_FitMe.xlsx
+++ b/Docs/Specifications_FitMe.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>When reading for the colum there was more than 1 id with the filtered value</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Try Removing Top Failed</t>
+  </si>
+  <si>
+    <t>0x0006</t>
+  </si>
+  <si>
+    <t>Unable to close the DB connection</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,6 +532,17 @@
       </c>
       <c r="C7" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating readmes, create DataBase Design
</commit_message>
<xml_diff>
--- a/Docs/Specifications_FitMe.xlsx
+++ b/Docs/Specifications_FitMe.xlsx
@@ -25,75 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
-  <si>
-    <t>When reading for the colum there was more than 1 id with the filtered value</t>
-  </si>
-  <si>
-    <t>TopModel</t>
-  </si>
-  <si>
-    <t>0x0000</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">completion interval </t>
   </si>
   <si>
-    <t>0x0001</t>
-  </si>
-  <si>
-    <t>UserModel</t>
-  </si>
-  <si>
-    <t>When signing in we found repeat emails in DB</t>
-  </si>
-  <si>
-    <t>0x0002</t>
-  </si>
-  <si>
-    <t>Failure displaying user profile because user is incomplete</t>
-  </si>
-  <si>
-    <t>UserProfile.aspx</t>
-  </si>
-  <si>
-    <t>0x0003</t>
-  </si>
-  <si>
-    <t>Database is not responding</t>
-  </si>
-  <si>
-    <t>DataBase.cs</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>0x0004</t>
-  </si>
-  <si>
-    <t>0x0005</t>
-  </si>
-  <si>
-    <t>TopModel.cs</t>
-  </si>
-  <si>
-    <t>Failed to ReadFromTable,</t>
-  </si>
-  <si>
-    <t>Try Removing Top Failed</t>
-  </si>
-  <si>
-    <t>0x0006</t>
-  </si>
-  <si>
-    <t>Unable to close the DB connection</t>
+    <t>Tracked in FitMe/Documentation/ExceptionList.md</t>
   </si>
 </sst>
 </file>
@@ -445,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,92 +394,9 @@
     <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -565,7 +419,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>200</v>

</xml_diff>